<commit_message>
testing new ipmopat package
</commit_message>
<xml_diff>
--- a/data/raw/ANT-compost-lettuce.xlsx
+++ b/data/raw/ANT-compost-lettuce.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au757887\PC_documents\_git-it\ghproj_ADOPTOPAT\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F1C61D-DEF5-49E3-A822-A6AB15BFC33B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F095DA-607E-4568-BD84-8F66BE0E5BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{D6B343A2-8466-44D0-A9FB-0D00DB7A8F67}"/>
+    <workbookView xWindow="38775" yWindow="9345" windowWidth="17280" windowHeight="8880" xr2:uid="{D6B343A2-8466-44D0-A9FB-0D00DB7A8F67}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="29">
-  <si>
-    <t>losses</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="21">
   <si>
     <t>health and safety</t>
   </si>
@@ -56,18 +53,9 @@
     <t>coordination requirements</t>
   </si>
   <si>
-    <t>impact category</t>
-  </si>
-  <si>
-    <t>rating</t>
-  </si>
-  <si>
     <t>H</t>
   </si>
   <si>
-    <t>confidence</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -80,49 +68,37 @@
     <t>title</t>
   </si>
   <si>
-    <t>Maintaining crop value</t>
-  </si>
-  <si>
-    <t>Reducing health and safety risks</t>
-  </si>
-  <si>
-    <t>Minimizing direct costs</t>
-  </si>
-  <si>
-    <t>Minimizing environmental impacts</t>
-  </si>
-  <si>
-    <t>Minimizing time and management demands</t>
-  </si>
-  <si>
-    <t>Immediate usability</t>
-  </si>
-  <si>
     <t>medium impact</t>
   </si>
   <si>
     <t>weight</t>
   </si>
   <si>
-    <t>Taken from the elicitation data coming from ANT-lettuce-compost</t>
-  </si>
-  <si>
-    <t>Weights are assumed from EUCLID default values</t>
-  </si>
-  <si>
     <t>12.5</t>
   </si>
   <si>
     <t>6.25</t>
   </si>
   <si>
-    <t>scenario</t>
-  </si>
-  <si>
-    <t>ADOPT</t>
-  </si>
-  <si>
-    <t>CCP</t>
+    <t>short</t>
+  </si>
+  <si>
+    <t>ccp_rating</t>
+  </si>
+  <si>
+    <t>ccp_confidence</t>
+  </si>
+  <si>
+    <t>ipm_rating</t>
+  </si>
+  <si>
+    <t>ipm_confidence</t>
+  </si>
+  <si>
+    <t>crop value</t>
+  </si>
+  <si>
+    <t>ANT - compost on lettuce</t>
   </si>
 </sst>
 </file>
@@ -494,288 +470,172 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B047F181-6D76-47D3-A6DA-08B978DD20BB}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="36.5546875" customWidth="1"/>
-    <col min="4" max="4" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.44140625" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="105.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="D6" t="s">
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
         <v>6</v>
-      </c>
-      <c r="E6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>50</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
-        <v>11</v>
       </c>
       <c r="F7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>50</v>
-      </c>
-      <c r="B13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" t="s">
-        <v>0</v>
-      </c>
-      <c r="E13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" t="s">
-        <v>4</v>
-      </c>
-      <c r="E17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" t="s">
-        <v>10</v>
+      <c r="G7" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>